<commit_message>
Fixed U12 from D2PAK to DPAK
</commit_message>
<xml_diff>
--- a/hardware/hydra/bom.xlsx
+++ b/hardware/hydra/bom.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="1080" windowWidth="1845" windowHeight="15195" tabRatio="500"/>
+    <workbookView xWindow="200" yWindow="1080" windowWidth="35800" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Detailed" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,19 @@
     <definedName name="partslist" localSheetId="1">Condensed!$A$1:$C$56</definedName>
     <definedName name="partslist" localSheetId="0">Detailed!$A$3:$C$106</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="partslist" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10017" firstRow="7" sourceFile="Home:Users:terahz:Documents:eagle:hydra-reef-read-only:hardware:hydra:partslist.txt" delimited="0">
+    <textPr fileType="mac" firstRow="7" sourceFile="Home:Users:terahz:Documents:eagle:hydra-reef-read-only:hardware:hydra:partslist.txt" delimited="0">
       <textFields count="6">
         <textField/>
         <textField position="9"/>
@@ -33,7 +38,7 @@
     </textPr>
   </connection>
   <connection id="2" name="partslist1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10017" firstRow="7" sourceFile="Home:Users:terahz:Documents:eagle:hydra-reef-read-only:hardware:hydra:partslist.txt" delimited="0">
+    <textPr fileType="mac" firstRow="7" sourceFile="Home:Users:terahz:Documents:eagle:hydra-reef-read-only:hardware:hydra:partslist.txt" delimited="0">
       <textFields count="6">
         <textField/>
         <textField position="9"/>
@@ -812,12 +817,6 @@
     <t>Optional. Protects your Ics.</t>
   </si>
   <si>
-    <t>511-L7805ABD2T-TR</t>
-  </si>
-  <si>
-    <t>Alternate: Any 7805 in same package, i.e. 511-L7805CD2T-TR</t>
-  </si>
-  <si>
     <t>A32260-ND</t>
   </si>
   <si>
@@ -830,9 +829,6 @@
     <t>3M5473-ND</t>
   </si>
   <si>
-    <t>497-1170-1-ND</t>
-  </si>
-  <si>
     <t>ICL7660CPA-ND</t>
   </si>
   <si>
@@ -1023,18 +1019,28 @@
   </si>
   <si>
     <t>BL01RN1A</t>
+  </si>
+  <si>
+    <t>MC7805CDTGOS-ND</t>
+  </si>
+  <si>
+    <t>863-MC7805CDTRKG</t>
+  </si>
+  <si>
+    <t>Alternate: Any 7805 in same package (DPAK)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1046,6 +1052,24 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1084,8 +1108,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1111,7 +1143,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1516,27 +1556,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="126.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="126.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25">
+    <row r="1" spans="1:7" ht="23">
       <c r="A1" s="9" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1565,7 +1605,7 @@
         <v>238</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1684,7 +1724,7 @@
         <v>168</v>
       </c>
       <c r="E8" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -1705,7 +1745,7 @@
         <v>168</v>
       </c>
       <c r="E9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -2065,7 +2105,7 @@
         <v>169</v>
       </c>
       <c r="E26" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -2233,7 +2273,7 @@
         <v>171</v>
       </c>
       <c r="E34" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="0"/>
@@ -2275,10 +2315,10 @@
         <v>170</v>
       </c>
       <c r="E36" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F36" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="0"/>
@@ -2362,10 +2402,10 @@
         <v>170</v>
       </c>
       <c r="E40" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F40" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -2446,7 +2486,7 @@
         <v>59</v>
       </c>
       <c r="F45" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="0"/>
@@ -2668,13 +2708,13 @@
         <v>71</v>
       </c>
       <c r="C58" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D58" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E58" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="0"/>
@@ -2692,7 +2732,7 @@
         <v>177</v>
       </c>
       <c r="E59" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F59" t="s">
         <v>240</v>
@@ -2713,7 +2753,7 @@
         <v>178</v>
       </c>
       <c r="E60" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="0"/>
@@ -2734,7 +2774,7 @@
         <v>179</v>
       </c>
       <c r="E61" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
@@ -2755,7 +2795,7 @@
         <v>179</v>
       </c>
       <c r="E62" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="0"/>
@@ -2776,7 +2816,7 @@
         <v>180</v>
       </c>
       <c r="E63" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="0"/>
@@ -2797,7 +2837,7 @@
         <v>181</v>
       </c>
       <c r="E64" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="0"/>
@@ -2818,7 +2858,7 @@
         <v>181</v>
       </c>
       <c r="E65" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="0"/>
@@ -2839,7 +2879,7 @@
         <v>182</v>
       </c>
       <c r="E66" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="0"/>
@@ -2860,7 +2900,7 @@
         <v>183</v>
       </c>
       <c r="E67" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="0"/>
@@ -2881,7 +2921,7 @@
         <v>183</v>
       </c>
       <c r="E68" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" ref="G68:G116" si="1">IF(ISBLANK(E68),"",CONCATENATE("1,",E68,",",A68))</f>
@@ -2902,7 +2942,7 @@
         <v>184</v>
       </c>
       <c r="E69" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
@@ -2923,7 +2963,7 @@
         <v>182</v>
       </c>
       <c r="E70" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
@@ -2944,7 +2984,7 @@
         <v>182</v>
       </c>
       <c r="E71" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
@@ -2965,7 +3005,7 @@
         <v>182</v>
       </c>
       <c r="E72" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
@@ -2986,7 +3026,7 @@
         <v>183</v>
       </c>
       <c r="E73" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
@@ -3007,7 +3047,7 @@
         <v>183</v>
       </c>
       <c r="E74" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
@@ -3028,7 +3068,7 @@
         <v>183</v>
       </c>
       <c r="E75" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" si="1"/>
@@ -3049,7 +3089,7 @@
         <v>185</v>
       </c>
       <c r="E76" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="1"/>
@@ -3070,7 +3110,7 @@
         <v>186</v>
       </c>
       <c r="E77" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="1"/>
@@ -3091,7 +3131,7 @@
         <v>183</v>
       </c>
       <c r="E78" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="1"/>
@@ -3112,7 +3152,7 @@
         <v>186</v>
       </c>
       <c r="E79" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="1"/>
@@ -3133,7 +3173,7 @@
         <v>186</v>
       </c>
       <c r="E80" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="1"/>
@@ -3154,7 +3194,7 @@
         <v>185</v>
       </c>
       <c r="E81" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="1"/>
@@ -3175,7 +3215,7 @@
         <v>187</v>
       </c>
       <c r="E82" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="1"/>
@@ -3196,7 +3236,7 @@
         <v>188</v>
       </c>
       <c r="E83" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="1"/>
@@ -3217,7 +3257,7 @@
         <v>187</v>
       </c>
       <c r="E84" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="1"/>
@@ -3238,7 +3278,7 @@
         <v>187</v>
       </c>
       <c r="E85" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="1"/>
@@ -3259,7 +3299,7 @@
         <v>189</v>
       </c>
       <c r="E86" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G86" t="str">
         <f t="shared" si="1"/>
@@ -3280,7 +3320,7 @@
         <v>190</v>
       </c>
       <c r="E87" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" si="1"/>
@@ -3301,7 +3341,7 @@
         <v>187</v>
       </c>
       <c r="E88" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="1"/>
@@ -3322,7 +3362,7 @@
         <v>191</v>
       </c>
       <c r="E89" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G89" t="str">
         <f t="shared" si="1"/>
@@ -3343,7 +3383,7 @@
         <v>192</v>
       </c>
       <c r="E90" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G90" t="str">
         <f t="shared" si="1"/>
@@ -3364,7 +3404,7 @@
         <v>193</v>
       </c>
       <c r="E91" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G91" t="str">
         <f t="shared" si="1"/>
@@ -3385,7 +3425,7 @@
         <v>193</v>
       </c>
       <c r="E92" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G92" t="str">
         <f t="shared" si="1"/>
@@ -3406,7 +3446,7 @@
         <v>194</v>
       </c>
       <c r="E93" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G93" t="str">
         <f t="shared" si="1"/>
@@ -3466,7 +3506,7 @@
         <v>196</v>
       </c>
       <c r="E96" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="1"/>
@@ -3487,7 +3527,7 @@
         <v>197</v>
       </c>
       <c r="E97" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G97" t="str">
         <f t="shared" si="1"/>
@@ -3508,7 +3548,7 @@
         <v>198</v>
       </c>
       <c r="E98" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" si="1"/>
@@ -3547,7 +3587,7 @@
         <v>199</v>
       </c>
       <c r="E100" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G100" t="str">
         <f t="shared" si="1"/>
@@ -3568,7 +3608,7 @@
         <v>200</v>
       </c>
       <c r="E101" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" si="1"/>
@@ -3607,7 +3647,7 @@
         <v>202</v>
       </c>
       <c r="E103" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="1"/>
@@ -3640,17 +3680,17 @@
         <v>159</v>
       </c>
       <c r="D105" t="s">
-        <v>254</v>
+        <v>323</v>
       </c>
       <c r="E105" t="s">
-        <v>260</v>
+        <v>322</v>
       </c>
       <c r="F105" t="s">
-        <v>255</v>
+        <v>324</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="1"/>
-        <v>1,497-1170-1-ND,U12</v>
+        <v>1,MC7805CDTGOS-ND,U12</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -3667,7 +3707,7 @@
         <v>204</v>
       </c>
       <c r="E106" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G106" t="str">
         <f t="shared" si="1"/>
@@ -3679,16 +3719,16 @@
         <v>215</v>
       </c>
       <c r="B107" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C107" t="s">
         <v>133</v>
       </c>
       <c r="D107" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E107" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F107" t="s">
         <v>253</v>
@@ -3703,16 +3743,16 @@
         <v>216</v>
       </c>
       <c r="B108" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C108" t="s">
         <v>133</v>
       </c>
       <c r="D108" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E108" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F108" t="s">
         <v>253</v>
@@ -3736,7 +3776,7 @@
         <v>224</v>
       </c>
       <c r="E109" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F109" t="s">
         <v>253</v>
@@ -3760,7 +3800,7 @@
         <v>225</v>
       </c>
       <c r="E110" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F110" t="s">
         <v>253</v>
@@ -3775,16 +3815,16 @@
         <v>219</v>
       </c>
       <c r="B111" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C111" t="s">
         <v>133</v>
       </c>
       <c r="D111" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E111" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F111" t="s">
         <v>253</v>
@@ -3808,7 +3848,7 @@
         <v>226</v>
       </c>
       <c r="E112" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F112" t="s">
         <v>253</v>
@@ -3832,7 +3872,7 @@
         <v>224</v>
       </c>
       <c r="E113" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F113" t="s">
         <v>253</v>
@@ -3856,7 +3896,7 @@
         <v>226</v>
       </c>
       <c r="E114" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F114" t="s">
         <v>253</v>
@@ -3880,7 +3920,7 @@
         <v>226</v>
       </c>
       <c r="E115" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F115" t="s">
         <v>253</v>
@@ -3917,31 +3957,36 @@
   <ignoredErrors>
     <ignoredError sqref="G41:G57 G95 G99" emptyCellReference="1"/>
   </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G181"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="23.875" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" customWidth="1"/>
     <col min="7" max="7" width="72" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -3979,7 +4024,7 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1">
@@ -3999,7 +4044,7 @@
         <v>208</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4016,10 +4061,10 @@
         <v>168</v>
       </c>
       <c r="E5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F5" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1">
@@ -4062,7 +4107,7 @@
         <v>212</v>
       </c>
       <c r="F7" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="2" customFormat="1">
@@ -4079,7 +4124,7 @@
         <v>169</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>31</v>
@@ -4102,7 +4147,7 @@
         <v>209</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="2" customFormat="1">
@@ -4119,7 +4164,7 @@
         <v>171</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>42</v>
@@ -4139,13 +4184,13 @@
         <v>170</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="2" customFormat="1">
@@ -4196,7 +4241,7 @@
         <v>234</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4210,7 +4255,7 @@
         <v>230</v>
       </c>
       <c r="F15" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="2" customFormat="1">
@@ -4227,7 +4272,7 @@
         <v>58</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="4" customFormat="1">
@@ -4258,7 +4303,7 @@
         <v>235</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4278,7 +4323,7 @@
         <v>68</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1">
@@ -4333,7 +4378,7 @@
         <v>236</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1">
@@ -4344,13 +4389,13 @@
         <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D23" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E23" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>70</v>
@@ -4367,7 +4412,7 @@
         <v>177</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>72</v>
@@ -4387,7 +4432,7 @@
         <v>178</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>74</v>
@@ -4407,10 +4452,10 @@
         <v>179</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="4" customFormat="1">
@@ -4427,7 +4472,7 @@
         <v>180</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>80</v>
@@ -4447,10 +4492,10 @@
         <v>181</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1">
@@ -4467,7 +4512,7 @@
         <v>182</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>86</v>
@@ -4487,10 +4532,10 @@
         <v>183</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="4" customFormat="1">
@@ -4507,7 +4552,7 @@
         <v>184</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>90</v>
@@ -4527,10 +4572,10 @@
         <v>182</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="4" customFormat="1">
@@ -4547,10 +4592,10 @@
         <v>183</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:7" s="2" customFormat="1">
@@ -4567,10 +4612,10 @@
         <v>185</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="1:7" s="4" customFormat="1">
@@ -4587,10 +4632,10 @@
         <v>186</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:7" s="2" customFormat="1">
@@ -4607,7 +4652,7 @@
         <v>183</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>102</v>
@@ -4627,10 +4672,10 @@
         <v>187</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:7" s="2" customFormat="1">
@@ -4647,7 +4692,7 @@
         <v>188</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>108</v>
@@ -4667,7 +4712,7 @@
         <v>189</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>112</v>
@@ -4687,7 +4732,7 @@
         <v>190</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>114</v>
@@ -4707,7 +4752,7 @@
         <v>191</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>117</v>
@@ -4727,7 +4772,7 @@
         <v>192</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>119</v>
@@ -4747,10 +4792,10 @@
         <v>193</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="2" customFormat="1">
@@ -4767,7 +4812,7 @@
         <v>194</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>125</v>
@@ -4804,7 +4849,7 @@
         <v>133</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>252</v>
@@ -4824,7 +4869,7 @@
         <v>196</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>135</v>
@@ -4844,7 +4889,7 @@
         <v>197</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>138</v>
@@ -4864,7 +4909,7 @@
         <v>198</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>141</v>
@@ -4884,7 +4929,7 @@
         <v>199</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>145</v>
@@ -4904,7 +4949,7 @@
         <v>200</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>148</v>
@@ -4941,7 +4986,7 @@
         <v>202</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>153</v>
@@ -4971,17 +5016,17 @@
       <c r="C55" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>260</v>
+      <c r="D55" t="s">
+        <v>323</v>
+      </c>
+      <c r="E55" t="s">
+        <v>322</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="G55" s="4" t="s">
-        <v>255</v>
+      <c r="G55" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="2" customFormat="1">
@@ -4998,7 +5043,7 @@
         <v>204</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>160</v>
@@ -5009,19 +5054,19 @@
         <v>3</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>133</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G57" s="4" t="s">
         <v>253</v>
@@ -5041,10 +5086,10 @@
         <v>224</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>253</v>
@@ -5064,7 +5109,7 @@
         <v>225</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>218</v>
@@ -5087,10 +5132,10 @@
         <v>226</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>253</v>
@@ -5474,7 +5519,11 @@
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>